<commit_message>
Check for missing 'With Properties' in assertion tables
And improve error message of the equivalent check for setup /
given tables
</commit_message>
<xml_diff>
--- a/Test/TestExcelFiles/NoHeadersForTable/NoHeadersForTable.xlsx
+++ b/Test/TestExcelFiles/NoHeadersForTable/NoHeadersForTable.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cburge\Documents\repos\customer-tests-excel\Test\TestExcelFiles\NoHeadersForTable\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{BC316742-0727-4002-ADFB-917FC13E252D}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{1141951F-00C6-4631-92CE-2500078E3F34}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{93574C7F-CD34-4A26-A791-2CAAC18DAAC8}"/>
   </bookViews>
@@ -114,7 +114,110 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="13">
+  <dxfs count="26">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -531,7 +634,7 @@
   <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>